<commit_message>
Prepared functions for class grouping
</commit_message>
<xml_diff>
--- a/data/testdata/SSG_SUBJECTS.xlsx
+++ b/data/testdata/SSG_SUBJECTS.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="162" uniqueCount="50">
   <si>
     <t xml:space="preserve">subject_ID</t>
   </si>
@@ -43,13 +43,133 @@
     <t xml:space="preserve">lesson_hours_ID</t>
   </si>
   <si>
-    <t xml:space="preserve">teacher_ID</t>
+    <t xml:space="preserve">teachers_ID</t>
   </si>
   <si>
     <t xml:space="preserve">classroom_ID</t>
   </si>
   <si>
     <t xml:space="preserve">NULL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[5, 9]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[8]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[9]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[15]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[45]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[32]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[6]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[51]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[46]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[13]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[23, 26]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[24, 19]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[27]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[18]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[14]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[19]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[20]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[21]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[2, 5]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[23]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[16]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[37]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[48]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[50]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[10, 13]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[14, 18]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[7]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[26]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[29]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[31, 33]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[45, 41]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[3]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[49]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[24]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[27, 32]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[30, 33]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[22]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[34]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[44]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[42]</t>
   </si>
 </sst>
 </file>
@@ -152,11 +272,11 @@
   </sheetPr>
   <dimension ref="A1:I52"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="B1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A11" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="H52" activeCellId="0" sqref="H52"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.578125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="10.42"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="16.57"/>
@@ -219,8 +339,8 @@
       <c r="G2" s="0" t="s">
         <v>9</v>
       </c>
-      <c r="H2" s="0" t="n">
-        <v>5</v>
+      <c r="H2" s="0" t="s">
+        <v>10</v>
       </c>
       <c r="I2" s="0" t="s">
         <v>9</v>
@@ -248,8 +368,8 @@
       <c r="G3" s="0" t="s">
         <v>9</v>
       </c>
-      <c r="H3" s="0" t="n">
-        <v>8</v>
+      <c r="H3" s="0" t="s">
+        <v>11</v>
       </c>
       <c r="I3" s="0" t="s">
         <v>9</v>
@@ -277,8 +397,8 @@
       <c r="G4" s="0" t="s">
         <v>9</v>
       </c>
-      <c r="H4" s="0" t="n">
-        <v>9</v>
+      <c r="H4" s="0" t="s">
+        <v>12</v>
       </c>
       <c r="I4" s="0" t="s">
         <v>9</v>
@@ -306,8 +426,8 @@
       <c r="G5" s="0" t="s">
         <v>9</v>
       </c>
-      <c r="H5" s="0" t="n">
-        <v>15</v>
+      <c r="H5" s="0" t="s">
+        <v>13</v>
       </c>
       <c r="I5" s="0" t="s">
         <v>9</v>
@@ -335,8 +455,8 @@
       <c r="G6" s="0" t="s">
         <v>9</v>
       </c>
-      <c r="H6" s="0" t="n">
-        <v>45</v>
+      <c r="H6" s="0" t="s">
+        <v>14</v>
       </c>
       <c r="I6" s="0" t="s">
         <v>9</v>
@@ -364,8 +484,8 @@
       <c r="G7" s="0" t="s">
         <v>9</v>
       </c>
-      <c r="H7" s="0" t="n">
-        <v>32</v>
+      <c r="H7" s="0" t="s">
+        <v>15</v>
       </c>
       <c r="I7" s="0" t="s">
         <v>9</v>
@@ -393,8 +513,8 @@
       <c r="G8" s="0" t="s">
         <v>9</v>
       </c>
-      <c r="H8" s="0" t="n">
-        <v>6</v>
+      <c r="H8" s="0" t="s">
+        <v>16</v>
       </c>
       <c r="I8" s="0" t="s">
         <v>9</v>
@@ -422,8 +542,8 @@
       <c r="G9" s="0" t="s">
         <v>9</v>
       </c>
-      <c r="H9" s="0" t="n">
-        <v>51</v>
+      <c r="H9" s="0" t="s">
+        <v>17</v>
       </c>
       <c r="I9" s="0" t="s">
         <v>9</v>
@@ -451,8 +571,8 @@
       <c r="G10" s="0" t="s">
         <v>9</v>
       </c>
-      <c r="H10" s="0" t="n">
-        <v>46</v>
+      <c r="H10" s="0" t="s">
+        <v>18</v>
       </c>
       <c r="I10" s="0" t="s">
         <v>9</v>
@@ -480,8 +600,8 @@
       <c r="G11" s="0" t="s">
         <v>9</v>
       </c>
-      <c r="H11" s="0" t="n">
-        <v>13</v>
+      <c r="H11" s="0" t="s">
+        <v>19</v>
       </c>
       <c r="I11" s="0" t="s">
         <v>9</v>
@@ -509,8 +629,8 @@
       <c r="G12" s="0" t="s">
         <v>9</v>
       </c>
-      <c r="H12" s="0" t="n">
-        <v>23</v>
+      <c r="H12" s="0" t="s">
+        <v>20</v>
       </c>
       <c r="I12" s="0" t="s">
         <v>9</v>
@@ -538,8 +658,8 @@
       <c r="G13" s="0" t="s">
         <v>9</v>
       </c>
-      <c r="H13" s="0" t="n">
-        <v>24</v>
+      <c r="H13" s="0" t="s">
+        <v>21</v>
       </c>
       <c r="I13" s="0" t="s">
         <v>9</v>
@@ -567,8 +687,8 @@
       <c r="G14" s="0" t="s">
         <v>9</v>
       </c>
-      <c r="H14" s="0" t="n">
-        <v>27</v>
+      <c r="H14" s="0" t="s">
+        <v>22</v>
       </c>
       <c r="I14" s="0" t="s">
         <v>9</v>
@@ -596,8 +716,8 @@
       <c r="G15" s="0" t="s">
         <v>9</v>
       </c>
-      <c r="H15" s="0" t="n">
-        <v>18</v>
+      <c r="H15" s="0" t="s">
+        <v>23</v>
       </c>
       <c r="I15" s="0" t="s">
         <v>9</v>
@@ -625,8 +745,8 @@
       <c r="G16" s="0" t="s">
         <v>9</v>
       </c>
-      <c r="H16" s="0" t="n">
-        <v>14</v>
+      <c r="H16" s="0" t="s">
+        <v>24</v>
       </c>
       <c r="I16" s="0" t="s">
         <v>9</v>
@@ -654,8 +774,8 @@
       <c r="G17" s="0" t="s">
         <v>9</v>
       </c>
-      <c r="H17" s="0" t="n">
-        <v>19</v>
+      <c r="H17" s="0" t="s">
+        <v>25</v>
       </c>
       <c r="I17" s="0" t="s">
         <v>9</v>
@@ -683,8 +803,8 @@
       <c r="G18" s="0" t="s">
         <v>9</v>
       </c>
-      <c r="H18" s="0" t="n">
-        <v>20</v>
+      <c r="H18" s="0" t="s">
+        <v>26</v>
       </c>
       <c r="I18" s="0" t="s">
         <v>9</v>
@@ -712,8 +832,8 @@
       <c r="G19" s="0" t="s">
         <v>9</v>
       </c>
-      <c r="H19" s="0" t="n">
-        <v>21</v>
+      <c r="H19" s="0" t="s">
+        <v>27</v>
       </c>
       <c r="I19" s="0" t="s">
         <v>9</v>
@@ -741,8 +861,8 @@
       <c r="G20" s="0" t="s">
         <v>9</v>
       </c>
-      <c r="H20" s="0" t="n">
-        <v>2</v>
+      <c r="H20" s="0" t="s">
+        <v>28</v>
       </c>
       <c r="I20" s="0" t="s">
         <v>9</v>
@@ -770,8 +890,8 @@
       <c r="G21" s="0" t="s">
         <v>9</v>
       </c>
-      <c r="H21" s="0" t="n">
-        <v>23</v>
+      <c r="H21" s="0" t="s">
+        <v>29</v>
       </c>
       <c r="I21" s="0" t="s">
         <v>9</v>
@@ -799,8 +919,8 @@
       <c r="G22" s="0" t="s">
         <v>9</v>
       </c>
-      <c r="H22" s="0" t="n">
-        <v>6</v>
+      <c r="H22" s="0" t="s">
+        <v>16</v>
       </c>
       <c r="I22" s="0" t="s">
         <v>9</v>
@@ -828,8 +948,8 @@
       <c r="G23" s="0" t="s">
         <v>9</v>
       </c>
-      <c r="H23" s="0" t="n">
-        <v>8</v>
+      <c r="H23" s="0" t="s">
+        <v>11</v>
       </c>
       <c r="I23" s="0" t="s">
         <v>9</v>
@@ -857,8 +977,8 @@
       <c r="G24" s="0" t="s">
         <v>9</v>
       </c>
-      <c r="H24" s="0" t="n">
-        <v>13</v>
+      <c r="H24" s="0" t="s">
+        <v>19</v>
       </c>
       <c r="I24" s="0" t="s">
         <v>9</v>
@@ -886,8 +1006,8 @@
       <c r="G25" s="0" t="s">
         <v>9</v>
       </c>
-      <c r="H25" s="0" t="n">
-        <v>16</v>
+      <c r="H25" s="0" t="s">
+        <v>30</v>
       </c>
       <c r="I25" s="0" t="s">
         <v>9</v>
@@ -915,8 +1035,8 @@
       <c r="G26" s="0" t="s">
         <v>9</v>
       </c>
-      <c r="H26" s="0" t="n">
-        <v>37</v>
+      <c r="H26" s="0" t="s">
+        <v>31</v>
       </c>
       <c r="I26" s="0" t="s">
         <v>9</v>
@@ -944,8 +1064,8 @@
       <c r="G27" s="0" t="s">
         <v>9</v>
       </c>
-      <c r="H27" s="0" t="n">
-        <v>48</v>
+      <c r="H27" s="0" t="s">
+        <v>32</v>
       </c>
       <c r="I27" s="0" t="s">
         <v>9</v>
@@ -973,8 +1093,8 @@
       <c r="G28" s="0" t="s">
         <v>9</v>
       </c>
-      <c r="H28" s="0" t="n">
-        <v>50</v>
+      <c r="H28" s="0" t="s">
+        <v>33</v>
       </c>
       <c r="I28" s="0" t="s">
         <v>9</v>
@@ -1002,8 +1122,8 @@
       <c r="G29" s="0" t="s">
         <v>9</v>
       </c>
-      <c r="H29" s="0" t="n">
-        <v>13</v>
+      <c r="H29" s="0" t="s">
+        <v>34</v>
       </c>
       <c r="I29" s="0" t="s">
         <v>9</v>
@@ -1031,8 +1151,8 @@
       <c r="G30" s="0" t="s">
         <v>9</v>
       </c>
-      <c r="H30" s="0" t="n">
-        <v>14</v>
+      <c r="H30" s="0" t="s">
+        <v>35</v>
       </c>
       <c r="I30" s="0" t="s">
         <v>9</v>
@@ -1060,8 +1180,8 @@
       <c r="G31" s="0" t="s">
         <v>9</v>
       </c>
-      <c r="H31" s="0" t="n">
-        <v>16</v>
+      <c r="H31" s="0" t="s">
+        <v>30</v>
       </c>
       <c r="I31" s="0" t="s">
         <v>9</v>
@@ -1089,8 +1209,8 @@
       <c r="G32" s="0" t="s">
         <v>9</v>
       </c>
-      <c r="H32" s="0" t="n">
-        <v>7</v>
+      <c r="H32" s="0" t="s">
+        <v>36</v>
       </c>
       <c r="I32" s="0" t="s">
         <v>9</v>
@@ -1118,8 +1238,8 @@
       <c r="G33" s="0" t="s">
         <v>9</v>
       </c>
-      <c r="H33" s="0" t="n">
-        <v>26</v>
+      <c r="H33" s="0" t="s">
+        <v>37</v>
       </c>
       <c r="I33" s="0" t="s">
         <v>9</v>
@@ -1147,8 +1267,8 @@
       <c r="G34" s="0" t="s">
         <v>9</v>
       </c>
-      <c r="H34" s="0" t="n">
-        <v>23</v>
+      <c r="H34" s="0" t="s">
+        <v>29</v>
       </c>
       <c r="I34" s="0" t="s">
         <v>9</v>
@@ -1176,8 +1296,8 @@
       <c r="G35" s="0" t="s">
         <v>9</v>
       </c>
-      <c r="H35" s="0" t="n">
-        <v>29</v>
+      <c r="H35" s="0" t="s">
+        <v>38</v>
       </c>
       <c r="I35" s="0" t="s">
         <v>9</v>
@@ -1205,8 +1325,8 @@
       <c r="G36" s="0" t="s">
         <v>9</v>
       </c>
-      <c r="H36" s="0" t="n">
-        <v>31</v>
+      <c r="H36" s="0" t="s">
+        <v>39</v>
       </c>
       <c r="I36" s="0" t="s">
         <v>9</v>
@@ -1234,8 +1354,8 @@
       <c r="G37" s="0" t="s">
         <v>9</v>
       </c>
-      <c r="H37" s="0" t="n">
-        <v>41</v>
+      <c r="H37" s="0" t="s">
+        <v>40</v>
       </c>
       <c r="I37" s="0" t="s">
         <v>9</v>
@@ -1263,8 +1383,8 @@
       <c r="G38" s="0" t="s">
         <v>9</v>
       </c>
-      <c r="H38" s="0" t="n">
-        <v>19</v>
+      <c r="H38" s="0" t="s">
+        <v>25</v>
       </c>
       <c r="I38" s="0" t="s">
         <v>9</v>
@@ -1292,8 +1412,8 @@
       <c r="G39" s="0" t="s">
         <v>9</v>
       </c>
-      <c r="H39" s="0" t="n">
-        <v>3</v>
+      <c r="H39" s="0" t="s">
+        <v>41</v>
       </c>
       <c r="I39" s="0" t="s">
         <v>9</v>
@@ -1321,8 +1441,8 @@
       <c r="G40" s="0" t="s">
         <v>9</v>
       </c>
-      <c r="H40" s="0" t="n">
-        <v>49</v>
+      <c r="H40" s="0" t="s">
+        <v>42</v>
       </c>
       <c r="I40" s="0" t="s">
         <v>9</v>
@@ -1350,8 +1470,8 @@
       <c r="G41" s="0" t="s">
         <v>9</v>
       </c>
-      <c r="H41" s="0" t="n">
-        <v>51</v>
+      <c r="H41" s="0" t="s">
+        <v>17</v>
       </c>
       <c r="I41" s="0" t="s">
         <v>9</v>
@@ -1379,8 +1499,8 @@
       <c r="G42" s="0" t="s">
         <v>9</v>
       </c>
-      <c r="H42" s="0" t="n">
-        <v>16</v>
+      <c r="H42" s="0" t="s">
+        <v>30</v>
       </c>
       <c r="I42" s="0" t="s">
         <v>9</v>
@@ -1408,8 +1528,8 @@
       <c r="G43" s="0" t="s">
         <v>9</v>
       </c>
-      <c r="H43" s="0" t="n">
-        <v>24</v>
+      <c r="H43" s="0" t="s">
+        <v>43</v>
       </c>
       <c r="I43" s="0" t="s">
         <v>9</v>
@@ -1437,8 +1557,8 @@
       <c r="G44" s="0" t="s">
         <v>9</v>
       </c>
-      <c r="H44" s="0" t="n">
-        <v>27</v>
+      <c r="H44" s="0" t="s">
+        <v>22</v>
       </c>
       <c r="I44" s="0" t="s">
         <v>9</v>
@@ -1466,8 +1586,8 @@
       <c r="G45" s="0" t="s">
         <v>9</v>
       </c>
-      <c r="H45" s="0" t="n">
-        <v>29</v>
+      <c r="H45" s="0" t="s">
+        <v>38</v>
       </c>
       <c r="I45" s="0" t="s">
         <v>9</v>
@@ -1495,8 +1615,8 @@
       <c r="G46" s="0" t="s">
         <v>9</v>
       </c>
-      <c r="H46" s="0" t="n">
-        <v>32</v>
+      <c r="H46" s="0" t="s">
+        <v>44</v>
       </c>
       <c r="I46" s="0" t="s">
         <v>9</v>
@@ -1524,8 +1644,8 @@
       <c r="G47" s="0" t="s">
         <v>9</v>
       </c>
-      <c r="H47" s="0" t="n">
-        <v>33</v>
+      <c r="H47" s="0" t="s">
+        <v>45</v>
       </c>
       <c r="I47" s="0" t="s">
         <v>9</v>
@@ -1553,8 +1673,8 @@
       <c r="G48" s="0" t="s">
         <v>9</v>
       </c>
-      <c r="H48" s="0" t="n">
-        <v>22</v>
+      <c r="H48" s="0" t="s">
+        <v>46</v>
       </c>
       <c r="I48" s="0" t="s">
         <v>9</v>
@@ -1582,8 +1702,8 @@
       <c r="G49" s="0" t="s">
         <v>9</v>
       </c>
-      <c r="H49" s="0" t="n">
-        <v>34</v>
+      <c r="H49" s="0" t="s">
+        <v>47</v>
       </c>
       <c r="I49" s="0" t="s">
         <v>9</v>
@@ -1611,8 +1731,8 @@
       <c r="G50" s="0" t="s">
         <v>9</v>
       </c>
-      <c r="H50" s="0" t="n">
-        <v>37</v>
+      <c r="H50" s="0" t="s">
+        <v>31</v>
       </c>
       <c r="I50" s="0" t="s">
         <v>9</v>
@@ -1640,8 +1760,8 @@
       <c r="G51" s="0" t="s">
         <v>9</v>
       </c>
-      <c r="H51" s="0" t="n">
-        <v>44</v>
+      <c r="H51" s="0" t="s">
+        <v>48</v>
       </c>
       <c r="I51" s="0" t="s">
         <v>9</v>
@@ -1669,8 +1789,8 @@
       <c r="G52" s="0" t="s">
         <v>9</v>
       </c>
-      <c r="H52" s="0" t="n">
-        <v>42</v>
+      <c r="H52" s="0" t="s">
+        <v>49</v>
       </c>
       <c r="I52" s="0" t="s">
         <v>9</v>

</xml_diff>

<commit_message>
Changed add_classrooms to prioritize teachers classrooms
</commit_message>
<xml_diff>
--- a/data/testdata/SSG_SUBJECTS.xlsx
+++ b/data/testdata/SSG_SUBJECTS.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="215" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="215" uniqueCount="62">
   <si>
     <t xml:space="preserve">subject_ID</t>
   </si>
@@ -61,154 +61,145 @@
     <t xml:space="preserve">[5, 9]</t>
   </si>
   <si>
-    <t xml:space="preserve">[1, 2]</t>
+    <t xml:space="preserve">[1, 2, 3]</t>
   </si>
   <si>
     <t xml:space="preserve">[8]</t>
   </si>
   <si>
-    <t xml:space="preserve">[3]</t>
-  </si>
-  <si>
     <t xml:space="preserve">[9]</t>
   </si>
   <si>
+    <t xml:space="preserve">[15]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[45]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[32]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[6, 17]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[51, 40]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[46]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[36]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[23, 26]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[24, 19]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[27]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[18]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[14]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[19]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[20]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[21]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[2, 11]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[23, 4]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[6]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[12]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[13]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[16]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[37]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[48]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[50]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[10, 13]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[14, 18]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[38]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[7]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[35]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[23]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[29]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[31, 33]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[45, 41]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[3, 43]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[49]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[51]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[39, 25]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[24]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[28]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[27, 32]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[30, 33]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[22, 47]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[34]</t>
+  </si>
+  <si>
     <t xml:space="preserve">[1]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[15]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[45]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[32]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[6, 17]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[51, 40]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[46]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[36]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[23, 26]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[24, 19]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[27]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[18]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[14]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[19]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[20]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[21]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[2, 11]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[1, 3]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[23, 4]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[6]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[12]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[13]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[16]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[37]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[48]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[50]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[10, 13]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[14, 18]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[38]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[7]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[35]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[23]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[29]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[31, 33]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[45, 41]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[3, 43]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[49]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[51]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[39, 25]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[24]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[28]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[27, 32]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[30, 33]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[1,2]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[22, 47]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[34]</t>
   </si>
   <si>
     <t xml:space="preserve">[44]</t>
@@ -224,7 +215,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="7">
+  <fonts count="6">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -263,13 +254,6 @@
       <name val="Arial"/>
       <family val="0"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="238"/>
     </font>
   </fonts>
   <fills count="2">
@@ -314,7 +298,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -324,10 +308,6 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -351,12 +331,12 @@
   <dimension ref="A1:K52"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="K47" activeCellId="0" sqref="K47"/>
+      <selection pane="topLeft" activeCell="O49" activeCellId="0" sqref="O49"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.55078125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.5625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="20.36"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="20.37"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -461,7 +441,7 @@
         <v>3</v>
       </c>
       <c r="K3" s="0" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -487,7 +467,7 @@
         <v>11</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="I4" s="1" t="s">
         <v>11</v>
@@ -496,7 +476,7 @@
         <v>3</v>
       </c>
       <c r="K4" s="0" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -522,7 +502,7 @@
         <v>11</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="I5" s="1" t="s">
         <v>11</v>
@@ -531,7 +511,7 @@
         <v>2</v>
       </c>
       <c r="K5" s="0" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -557,7 +537,7 @@
         <v>11</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="I6" s="1" t="s">
         <v>11</v>
@@ -566,7 +546,7 @@
         <v>3</v>
       </c>
       <c r="K6" s="0" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -592,7 +572,7 @@
         <v>11</v>
       </c>
       <c r="H7" s="1" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="I7" s="1" t="s">
         <v>11</v>
@@ -601,7 +581,7 @@
         <v>4</v>
       </c>
       <c r="K7" s="0" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -627,7 +607,7 @@
         <v>11</v>
       </c>
       <c r="H8" s="1" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="I8" s="1" t="s">
         <v>11</v>
@@ -636,7 +616,7 @@
         <v>2</v>
       </c>
       <c r="K8" s="0" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -662,7 +642,7 @@
         <v>11</v>
       </c>
       <c r="H9" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="I9" s="1" t="s">
         <v>11</v>
@@ -671,7 +651,7 @@
         <v>2</v>
       </c>
       <c r="K9" s="0" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -697,7 +677,7 @@
         <v>11</v>
       </c>
       <c r="H10" s="1" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="I10" s="1" t="s">
         <v>11</v>
@@ -706,7 +686,7 @@
         <v>2</v>
       </c>
       <c r="K10" s="0" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -732,7 +712,7 @@
         <v>11</v>
       </c>
       <c r="H11" s="1" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="I11" s="1" t="s">
         <v>11</v>
@@ -741,7 +721,7 @@
         <v>3</v>
       </c>
       <c r="K11" s="0" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -767,7 +747,7 @@
         <v>11</v>
       </c>
       <c r="H12" s="1" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="I12" s="1" t="s">
         <v>11</v>
@@ -802,7 +782,7 @@
         <v>11</v>
       </c>
       <c r="H13" s="1" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="I13" s="1" t="s">
         <v>11</v>
@@ -837,7 +817,7 @@
         <v>11</v>
       </c>
       <c r="H14" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="I14" s="1" t="s">
         <v>11</v>
@@ -845,8 +825,8 @@
       <c r="J14" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="K14" s="3" t="s">
-        <v>17</v>
+      <c r="K14" s="0" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -872,7 +852,7 @@
         <v>11</v>
       </c>
       <c r="H15" s="1" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="I15" s="1" t="s">
         <v>11</v>
@@ -880,8 +860,8 @@
       <c r="J15" s="1" t="n">
         <v>3</v>
       </c>
-      <c r="K15" s="3" t="s">
-        <v>17</v>
+      <c r="K15" s="0" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -907,7 +887,7 @@
         <v>11</v>
       </c>
       <c r="H16" s="1" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="I16" s="1" t="s">
         <v>11</v>
@@ -915,8 +895,8 @@
       <c r="J16" s="1" t="n">
         <v>3</v>
       </c>
-      <c r="K16" s="3" t="s">
-        <v>17</v>
+      <c r="K16" s="0" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -942,7 +922,7 @@
         <v>11</v>
       </c>
       <c r="H17" s="1" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="I17" s="1" t="s">
         <v>11</v>
@@ -950,8 +930,8 @@
       <c r="J17" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="K17" s="3" t="s">
-        <v>17</v>
+      <c r="K17" s="0" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -977,7 +957,7 @@
         <v>11</v>
       </c>
       <c r="H18" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="I18" s="1" t="s">
         <v>11</v>
@@ -985,8 +965,8 @@
       <c r="J18" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="K18" s="3" t="s">
-        <v>17</v>
+      <c r="K18" s="0" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1012,7 +992,7 @@
         <v>11</v>
       </c>
       <c r="H19" s="1" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="I19" s="1" t="s">
         <v>11</v>
@@ -1020,8 +1000,8 @@
       <c r="J19" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="K19" s="3" t="s">
-        <v>15</v>
+      <c r="K19" s="0" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1047,7 +1027,7 @@
         <v>11</v>
       </c>
       <c r="H20" s="1" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="I20" s="1" t="s">
         <v>11</v>
@@ -1055,8 +1035,8 @@
       <c r="J20" s="1" t="n">
         <v>3</v>
       </c>
-      <c r="K20" s="3" t="s">
-        <v>34</v>
+      <c r="K20" s="0" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1082,7 +1062,7 @@
         <v>11</v>
       </c>
       <c r="H21" s="1" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="I21" s="1" t="s">
         <v>11</v>
@@ -1090,8 +1070,8 @@
       <c r="J21" s="1" t="n">
         <v>3</v>
       </c>
-      <c r="K21" s="3" t="s">
-        <v>17</v>
+      <c r="K21" s="0" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1117,7 +1097,7 @@
         <v>11</v>
       </c>
       <c r="H22" s="1" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="I22" s="1" t="s">
         <v>11</v>
@@ -1125,8 +1105,8 @@
       <c r="J22" s="1" t="n">
         <v>3</v>
       </c>
-      <c r="K22" s="3" t="s">
-        <v>17</v>
+      <c r="K22" s="0" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1152,7 +1132,7 @@
         <v>11</v>
       </c>
       <c r="H23" s="1" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="I23" s="1" t="s">
         <v>11</v>
@@ -1160,8 +1140,8 @@
       <c r="J23" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="K23" s="3" t="s">
-        <v>17</v>
+      <c r="K23" s="0" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1187,7 +1167,7 @@
         <v>11</v>
       </c>
       <c r="H24" s="1" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="I24" s="1" t="s">
         <v>11</v>
@@ -1195,8 +1175,8 @@
       <c r="J24" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="K24" s="3" t="s">
-        <v>17</v>
+      <c r="K24" s="0" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1222,7 +1202,7 @@
         <v>11</v>
       </c>
       <c r="H25" s="1" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="I25" s="1" t="s">
         <v>11</v>
@@ -1230,8 +1210,8 @@
       <c r="J25" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="K25" s="3" t="s">
-        <v>17</v>
+      <c r="K25" s="0" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1257,7 +1237,7 @@
         <v>11</v>
       </c>
       <c r="H26" s="1" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="I26" s="1" t="s">
         <v>11</v>
@@ -1265,8 +1245,8 @@
       <c r="J26" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="K26" s="3" t="s">
-        <v>17</v>
+      <c r="K26" s="0" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1292,7 +1272,7 @@
         <v>11</v>
       </c>
       <c r="H27" s="1" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="I27" s="1" t="s">
         <v>11</v>
@@ -1300,8 +1280,8 @@
       <c r="J27" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="K27" s="3" t="s">
-        <v>17</v>
+      <c r="K27" s="0" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1327,7 +1307,7 @@
         <v>11</v>
       </c>
       <c r="H28" s="1" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="I28" s="1" t="s">
         <v>11</v>
@@ -1335,8 +1315,8 @@
       <c r="J28" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="K28" s="3" t="s">
-        <v>17</v>
+      <c r="K28" s="0" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1362,7 +1342,7 @@
         <v>11</v>
       </c>
       <c r="H29" s="1" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="I29" s="1" t="s">
         <v>11</v>
@@ -1370,7 +1350,7 @@
       <c r="J29" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="K29" s="3" t="s">
+      <c r="K29" s="0" t="s">
         <v>13</v>
       </c>
     </row>
@@ -1397,7 +1377,7 @@
         <v>11</v>
       </c>
       <c r="H30" s="1" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="I30" s="1" t="s">
         <v>11</v>
@@ -1405,7 +1385,7 @@
       <c r="J30" s="1" t="n">
         <v>4</v>
       </c>
-      <c r="K30" s="3" t="s">
+      <c r="K30" s="0" t="s">
         <v>13</v>
       </c>
     </row>
@@ -1432,7 +1412,7 @@
         <v>11</v>
       </c>
       <c r="H31" s="1" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="I31" s="1" t="s">
         <v>11</v>
@@ -1440,8 +1420,8 @@
       <c r="J31" s="1" t="n">
         <v>4</v>
       </c>
-      <c r="K31" s="3" t="s">
-        <v>17</v>
+      <c r="K31" s="0" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1467,7 +1447,7 @@
         <v>11</v>
       </c>
       <c r="H32" s="1" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="I32" s="1" t="s">
         <v>11</v>
@@ -1475,8 +1455,8 @@
       <c r="J32" s="1" t="n">
         <v>3</v>
       </c>
-      <c r="K32" s="3" t="s">
-        <v>17</v>
+      <c r="K32" s="0" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1502,7 +1482,7 @@
         <v>11</v>
       </c>
       <c r="H33" s="1" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="I33" s="1" t="s">
         <v>11</v>
@@ -1510,8 +1490,8 @@
       <c r="J33" s="1" t="n">
         <v>3</v>
       </c>
-      <c r="K33" s="3" t="s">
-        <v>17</v>
+      <c r="K33" s="0" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1537,7 +1517,7 @@
         <v>11</v>
       </c>
       <c r="H34" s="1" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="I34" s="1" t="s">
         <v>11</v>
@@ -1545,8 +1525,8 @@
       <c r="J34" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="K34" s="3" t="s">
-        <v>17</v>
+      <c r="K34" s="0" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1572,7 +1552,7 @@
         <v>11</v>
       </c>
       <c r="H35" s="1" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="I35" s="1" t="s">
         <v>11</v>
@@ -1580,8 +1560,8 @@
       <c r="J35" s="1" t="n">
         <v>3</v>
       </c>
-      <c r="K35" s="3" t="s">
-        <v>17</v>
+      <c r="K35" s="0" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1607,7 +1587,7 @@
         <v>11</v>
       </c>
       <c r="H36" s="1" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="I36" s="1" t="s">
         <v>11</v>
@@ -1615,7 +1595,7 @@
       <c r="J36" s="1" t="n">
         <v>3</v>
       </c>
-      <c r="K36" s="3" t="s">
+      <c r="K36" s="0" t="s">
         <v>13</v>
       </c>
     </row>
@@ -1642,7 +1622,7 @@
         <v>11</v>
       </c>
       <c r="H37" s="1" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="I37" s="1" t="s">
         <v>11</v>
@@ -1650,7 +1630,7 @@
       <c r="J37" s="1" t="n">
         <v>3</v>
       </c>
-      <c r="K37" s="3" t="s">
+      <c r="K37" s="0" t="s">
         <v>13</v>
       </c>
     </row>
@@ -1677,7 +1657,7 @@
         <v>11</v>
       </c>
       <c r="H38" s="1" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="I38" s="1" t="s">
         <v>11</v>
@@ -1685,8 +1665,8 @@
       <c r="J38" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="K38" s="3" t="s">
-        <v>17</v>
+      <c r="K38" s="0" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1712,7 +1692,7 @@
         <v>11</v>
       </c>
       <c r="H39" s="1" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="I39" s="1" t="s">
         <v>11</v>
@@ -1720,8 +1700,8 @@
       <c r="J39" s="1" t="n">
         <v>3</v>
       </c>
-      <c r="K39" s="3" t="s">
-        <v>17</v>
+      <c r="K39" s="0" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1747,7 +1727,7 @@
         <v>11</v>
       </c>
       <c r="H40" s="1" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="I40" s="1" t="s">
         <v>11</v>
@@ -1755,8 +1735,8 @@
       <c r="J40" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="K40" s="3" t="s">
-        <v>17</v>
+      <c r="K40" s="0" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1782,7 +1762,7 @@
         <v>11</v>
       </c>
       <c r="H41" s="1" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="I41" s="1" t="s">
         <v>11</v>
@@ -1790,8 +1770,8 @@
       <c r="J41" s="1" t="n">
         <v>3</v>
       </c>
-      <c r="K41" s="3" t="s">
-        <v>17</v>
+      <c r="K41" s="0" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1817,7 +1797,7 @@
         <v>11</v>
       </c>
       <c r="H42" s="1" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="I42" s="1" t="s">
         <v>11</v>
@@ -1825,8 +1805,8 @@
       <c r="J42" s="1" t="n">
         <v>4</v>
       </c>
-      <c r="K42" s="3" t="s">
-        <v>17</v>
+      <c r="K42" s="0" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1852,7 +1832,7 @@
         <v>11</v>
       </c>
       <c r="H43" s="1" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="I43" s="1" t="s">
         <v>11</v>
@@ -1860,8 +1840,8 @@
       <c r="J43" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="K43" s="3" t="s">
-        <v>17</v>
+      <c r="K43" s="0" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1887,7 +1867,7 @@
         <v>11</v>
       </c>
       <c r="H44" s="1" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="I44" s="1" t="s">
         <v>11</v>
@@ -1895,8 +1875,8 @@
       <c r="J44" s="1" t="n">
         <v>3</v>
       </c>
-      <c r="K44" s="3" t="s">
-        <v>17</v>
+      <c r="K44" s="0" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1922,7 +1902,7 @@
         <v>11</v>
       </c>
       <c r="H45" s="1" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="I45" s="1" t="s">
         <v>11</v>
@@ -1930,8 +1910,8 @@
       <c r="J45" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="K45" s="3" t="s">
-        <v>17</v>
+      <c r="K45" s="0" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1957,7 +1937,7 @@
         <v>11</v>
       </c>
       <c r="H46" s="1" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="I46" s="1" t="s">
         <v>11</v>
@@ -1965,8 +1945,8 @@
       <c r="J46" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="K46" s="3" t="s">
-        <v>15</v>
+      <c r="K46" s="0" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1992,7 +1972,7 @@
         <v>11</v>
       </c>
       <c r="H47" s="1" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="I47" s="1" t="s">
         <v>11</v>
@@ -2000,8 +1980,8 @@
       <c r="J47" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="K47" s="3" t="s">
-        <v>60</v>
+      <c r="K47" s="0" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2027,7 +2007,7 @@
         <v>11</v>
       </c>
       <c r="H48" s="1" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="I48" s="1" t="s">
         <v>11</v>
@@ -2035,8 +2015,8 @@
       <c r="J48" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="K48" s="3" t="s">
-        <v>17</v>
+      <c r="K48" s="0" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2062,7 +2042,7 @@
         <v>11</v>
       </c>
       <c r="H49" s="1" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="I49" s="1" t="s">
         <v>11</v>
@@ -2070,8 +2050,8 @@
       <c r="J49" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="K49" s="3" t="s">
-        <v>17</v>
+      <c r="K49" s="0" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2097,7 +2077,7 @@
         <v>11</v>
       </c>
       <c r="H50" s="1" t="s">
-        <v>17</v>
+        <v>59</v>
       </c>
       <c r="I50" s="1" t="s">
         <v>11</v>
@@ -2105,8 +2085,8 @@
       <c r="J50" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="K50" s="3" t="s">
-        <v>17</v>
+      <c r="K50" s="0" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2132,7 +2112,7 @@
         <v>11</v>
       </c>
       <c r="H51" s="1" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="I51" s="1" t="s">
         <v>11</v>
@@ -2140,8 +2120,8 @@
       <c r="J51" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="K51" s="3" t="s">
-        <v>17</v>
+      <c r="K51" s="0" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2167,7 +2147,7 @@
         <v>11</v>
       </c>
       <c r="H52" s="1" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="I52" s="1" t="s">
         <v>11</v>
@@ -2175,8 +2155,8 @@
       <c r="J52" s="1" t="n">
         <v>3</v>
       </c>
-      <c r="K52" s="3" t="s">
-        <v>17</v>
+      <c r="K52" s="0" t="s">
+        <v>13</v>
       </c>
     </row>
   </sheetData>

</xml_diff>